<commit_message>
update dehalogenation ML naming
</commit_message>
<xml_diff>
--- a/Dehalogenation_colorimetric_assays/Experiment1/20240927_rep1_2_linearized_fluoride.xlsx
+++ b/Dehalogenation_colorimetric_assays/Experiment1/20240927_rep1_2_linearized_fluoride.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robinsse/Documents/github/biodefluorination-paper/machine_learning/data/machine_learning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robinsse/Documents/github/gut_microbe_defluorination_paper/Dehalogenation_colorimetric_assays/Experiment1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DCAEA9F-7FE9-964E-8CF2-0A853CFBF7F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2AE225A-1772-F74D-94B8-FE37E531F3EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2360" yWindow="500" windowWidth="26440" windowHeight="14080" xr2:uid="{3D85E17D-CCC7-684B-9790-2A98F5EB99A7}"/>
+    <workbookView xWindow="2360" yWindow="500" windowWidth="26440" windowHeight="14080" activeTab="1" xr2:uid="{3D85E17D-CCC7-684B-9790-2A98F5EB99A7}"/>
   </bookViews>
   <sheets>
-    <sheet name="rep3_linearized_fluoride" sheetId="1" r:id="rId1"/>
-    <sheet name="rep4_linearized_fluoride" sheetId="2" r:id="rId2"/>
+    <sheet name="rep1_linearized_fluoride" sheetId="1" r:id="rId1"/>
+    <sheet name="rep2_linearized_fluoride" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -109,9 +109,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -149,7 +149,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -255,7 +255,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -397,7 +397,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -407,7 +407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00CDFB34-0A9E-984D-9922-67E001B769C2}">
   <dimension ref="A1:AE8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AD5" sqref="AD5"/>
     </sheetView>
   </sheetViews>
@@ -1173,7 +1173,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A58BC798-A92A-6748-9B73-CB5422558775}">
   <dimension ref="A1:AE8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="W19" sqref="W19"/>
     </sheetView>
   </sheetViews>

</xml_diff>